<commit_message>
fix:ui request spesific accounts
</commit_message>
<xml_diff>
--- a/descriptive_statistics3.xlsx
+++ b/descriptive_statistics3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,55 +451,60 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>statuses_count</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>account_age_days</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ratio_statuses_count_per_age</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ratio_favorites_per_age</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>ratio_friends_per_followers</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>word_count</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>char_count</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>reputation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>description_word_count</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>description_character_count</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>avg_word</t>
         </is>
@@ -553,6 +558,9 @@
       <c r="O2" t="n">
         <v>1200</v>
       </c>
+      <c r="P2" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -561,46 +569,49 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9885.949166666667</v>
+        <v>10545.64333333333</v>
       </c>
       <c r="C3" t="n">
-        <v>464021.5875</v>
+        <v>337314.1641666667</v>
       </c>
       <c r="D3" t="n">
-        <v>4918.279166666666</v>
+        <v>4271.750833333334</v>
       </c>
       <c r="E3" t="n">
-        <v>21090.94</v>
+        <v>1.17659042009189e+17</v>
       </c>
       <c r="F3" t="n">
-        <v>3004.428333333333</v>
+        <v>24809.70416666667</v>
       </c>
       <c r="G3" t="n">
-        <v>6.638758527608017</v>
+        <v>3062.076666666667</v>
       </c>
       <c r="H3" t="n">
-        <v>3.764408148086102</v>
+        <v>7.888849631600142</v>
       </c>
       <c r="I3" t="n">
-        <v>2.303236456121974</v>
+        <v>3.631691511453875</v>
       </c>
       <c r="J3" t="n">
-        <v>10.00833333333333</v>
+        <v>2.709531735934661</v>
       </c>
       <c r="K3" t="n">
-        <v>66.40916666666666</v>
+        <v>9.783333333333333</v>
       </c>
       <c r="L3" t="n">
-        <v>0.625996425053439</v>
+        <v>64.5325</v>
       </c>
       <c r="M3" t="n">
-        <v>9.968333333333334</v>
+        <v>0.6331464341602853</v>
       </c>
       <c r="N3" t="n">
-        <v>57.26</v>
+        <v>9.484999999999999</v>
       </c>
       <c r="O3" t="n">
-        <v>5.516998734402787</v>
+        <v>55.565</v>
+      </c>
+      <c r="P3" t="n">
+        <v>5.78784525451346</v>
       </c>
     </row>
     <row r="4">
@@ -610,46 +621,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>24747.5436169763</v>
+        <v>25797.93519269118</v>
       </c>
       <c r="C4" t="n">
-        <v>3512307.087186476</v>
+        <v>1884400.071274768</v>
       </c>
       <c r="D4" t="n">
-        <v>43323.73081708406</v>
+        <v>51751.81873956503</v>
       </c>
       <c r="E4" t="n">
-        <v>63064.60654329111</v>
+        <v>2.92421216130287e+17</v>
       </c>
       <c r="F4" t="n">
-        <v>1020.857515320352</v>
+        <v>120484.1439924343</v>
       </c>
       <c r="G4" t="n">
-        <v>18.69330619702975</v>
+        <v>1001.046727804583</v>
       </c>
       <c r="H4" t="n">
-        <v>10.8666680524384</v>
+        <v>42.77300667365063</v>
       </c>
       <c r="I4" t="n">
-        <v>8.128659032914227</v>
+        <v>9.919048219479846</v>
       </c>
       <c r="J4" t="n">
-        <v>8.263282161604479</v>
+        <v>11.47763952068743</v>
       </c>
       <c r="K4" t="n">
-        <v>54.11512840146593</v>
+        <v>8.654891382502997</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3478819807735388</v>
+        <v>54.51399291254852</v>
       </c>
       <c r="M4" t="n">
-        <v>8.100329829190514</v>
+        <v>0.3534234229180773</v>
       </c>
       <c r="N4" t="n">
-        <v>46.50513957265613</v>
+        <v>7.960061378382896</v>
       </c>
       <c r="O4" t="n">
-        <v>4.87534698642562</v>
+        <v>46.97342717662045</v>
+      </c>
+      <c r="P4" t="n">
+        <v>7.045101187305121</v>
       </c>
     </row>
     <row r="5">
@@ -668,13 +682,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
+        <v>418</v>
+      </c>
+      <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="n">
-        <v>483</v>
-      </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -683,21 +697,24 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
       </c>
       <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
         <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>1</v>
       </c>
       <c r="N5" t="n">
         <v>1</v>
       </c>
       <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -708,46 +725,49 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>369.75</v>
+        <v>331.5</v>
       </c>
       <c r="C6" t="n">
-        <v>29.75</v>
+        <v>33</v>
       </c>
       <c r="D6" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="n">
-        <v>1331.75</v>
+        <v>94439953.25</v>
       </c>
       <c r="F6" t="n">
-        <v>2314.25</v>
+        <v>1363</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5115878262688949</v>
+        <v>2379.75</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1413919802790587</v>
+        <v>0.5013136288998358</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0008106616185106069</v>
+        <v>0.1124325701065373</v>
       </c>
       <c r="J6" t="n">
+        <v>0.0007312739345898219</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="L6" t="n">
+        <v>12</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.3137138574907887</v>
+      </c>
+      <c r="N6" t="n">
         <v>2</v>
       </c>
-      <c r="K6" t="n">
-        <v>15</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.32103019585071</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>13</v>
-      </c>
       <c r="O6" t="n">
-        <v>3.85042735042735</v>
+        <v>10.75</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3.657894736842105</v>
       </c>
     </row>
     <row r="7">
@@ -757,46 +777,49 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2057.5</v>
+        <v>2042.5</v>
       </c>
       <c r="C7" t="n">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D7" t="n">
-        <v>263</v>
+        <v>271.5</v>
       </c>
       <c r="E7" t="n">
-        <v>3945</v>
+        <v>377230939</v>
       </c>
       <c r="F7" t="n">
-        <v>3190.5</v>
+        <v>4436.5</v>
       </c>
       <c r="G7" t="n">
-        <v>1.418647408102463</v>
+        <v>3254.5</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6492877101774561</v>
+        <v>1.443625841750842</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6416122010706158</v>
+        <v>0.6632034452872573</v>
       </c>
       <c r="J7" t="n">
+        <v>0.4653561037105763</v>
+      </c>
+      <c r="K7" t="n">
         <v>8</v>
       </c>
-      <c r="K7" t="n">
-        <v>57</v>
-      </c>
       <c r="L7" t="n">
-        <v>0.6091574834735303</v>
+        <v>54</v>
       </c>
       <c r="M7" t="n">
+        <v>0.6824302202821855</v>
+      </c>
+      <c r="N7" t="n">
         <v>8</v>
       </c>
-      <c r="N7" t="n">
-        <v>49</v>
-      </c>
       <c r="O7" t="n">
-        <v>5.25</v>
+        <v>47</v>
+      </c>
+      <c r="P7" t="n">
+        <v>5.192307692307693</v>
       </c>
     </row>
     <row r="8">
@@ -806,46 +829,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7515</v>
+        <v>8328.25</v>
       </c>
       <c r="C8" t="n">
-        <v>8206.75</v>
+        <v>13282.25</v>
       </c>
       <c r="D8" t="n">
-        <v>857.75</v>
+        <v>813</v>
       </c>
       <c r="E8" t="n">
-        <v>15099</v>
+        <v>2338591177.25</v>
       </c>
       <c r="F8" t="n">
-        <v>3878.25</v>
+        <v>16481.5</v>
       </c>
       <c r="G8" t="n">
-        <v>5.277241459133752</v>
+        <v>3911</v>
       </c>
       <c r="H8" t="n">
-        <v>2.584223911879516</v>
+        <v>5.358665313230251</v>
       </c>
       <c r="I8" t="n">
-        <v>2.114971823770492</v>
+        <v>2.585386326599655</v>
       </c>
       <c r="J8" t="n">
+        <v>2.187619047619048</v>
+      </c>
+      <c r="K8" t="n">
         <v>16</v>
       </c>
-      <c r="K8" t="n">
-        <v>115</v>
-      </c>
       <c r="L8" t="n">
-        <v>0.9991899950255549</v>
+        <v>113</v>
       </c>
       <c r="M8" t="n">
+        <v>0.9992692604804158</v>
+      </c>
+      <c r="N8" t="n">
         <v>16</v>
       </c>
-      <c r="N8" t="n">
-        <v>99</v>
-      </c>
       <c r="O8" t="n">
-        <v>6.604761904761904</v>
+        <v>98</v>
+      </c>
+      <c r="P8" t="n">
+        <v>6.631578947368421</v>
       </c>
     </row>
     <row r="9">
@@ -855,46 +881,49 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>373633</v>
+        <v>354763</v>
       </c>
       <c r="C9" t="n">
-        <v>98161375</v>
+        <v>41478966</v>
       </c>
       <c r="D9" t="n">
-        <v>933476</v>
+        <v>1473166</v>
       </c>
       <c r="E9" t="n">
-        <v>1258100</v>
+        <v>1.118951206448181e+18</v>
       </c>
       <c r="F9" t="n">
-        <v>4972</v>
+        <v>2771910</v>
       </c>
       <c r="G9" t="n">
-        <v>337.2018225676762</v>
+        <v>5158</v>
       </c>
       <c r="H9" t="n">
-        <v>185.8958525345622</v>
+        <v>1062.034482758621</v>
       </c>
       <c r="I9" t="n">
-        <v>151.7142857142857</v>
+        <v>191.3500539374326</v>
       </c>
       <c r="J9" t="n">
-        <v>68</v>
+        <v>242.3333333333333</v>
       </c>
       <c r="K9" t="n">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="L9" t="n">
+        <v>165</v>
+      </c>
+      <c r="M9" t="n">
         <v>1</v>
       </c>
-      <c r="M9" t="n">
-        <v>34</v>
-      </c>
       <c r="N9" t="n">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="O9" t="n">
-        <v>63</v>
+        <v>156</v>
+      </c>
+      <c r="P9" t="n">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>